<commit_message>
Updating excel sheet with article
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Projects\phd\Article Searches\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFA2480-0EB4-4DEF-9526-72DEFADAA770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,87 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Search Term</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Pub. Year</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Blockchain-Enabled Federated learning
+for Enhanced Collaborative Intrusion Detection
+in Vehicular Edge Computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Author </t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Zakaria Abou El Houda</t>
+  </si>
+  <si>
+    <t>IEEE Xplore</t>
+  </si>
+  <si>
+    <t>("All Metadata":ai or artificial intelligence) AND ("All Metadata":federated learning)</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Intelligent Transportation Systems</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Intelligent Transportation Systems (ITSs) are transforming the global monitoring of road safety. These systems, including vehicular networks and transportation infrastructure, are vulnerable to several security issues, which could disrupt services and potentially cause harm to the users. It is crucial to establish robust security measures to protect against evolving attacks and ensure the safe and reliable operation of ITS. Artificial Intelligence (AI)-based Intrusion Detection Systems (IDS) are mainly used to enhance the security of ITS. The adoption of AI-based techniques to secure ITS against new emerging threats has been limited due to a lack of realistic and recent data on these types of attacks ( i.e., zero-day attacks). In this context, we introduce a novel Edge-based Framework that uses Federated Learning (FL) and blockchain to secure ITS against new emerging threats. In particular, our proposed framework consists of a novel distributed Edge-based architecture that allows multiple Edge nodes to securely collaborate while preserving their privacy; and (2) a decentralized and secure reputation system based on blockchain technology to maintain the reliability and trustworthiness of the FL process within the ITS; This system manages reputation data for individual nodes (such as vehicles), guaranteeing the integrity of the FL training process. Experiment results using the UNSW-NB15 dataset show that our proposed framework achieves high accuracy and F1 score (99%) in detecting new threats while ensuring the privacy and reliability of the whole ITS. These results demonstrate the effectiveness of our proposed framework in securing ITS.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +127,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +419,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="100.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{30F657E1-F976-457B-97E7-30705BFAEC49}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added articles to the Excel file
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1038064\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Projects\phd\Article Searches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648EE67D-29B9-4B2C-8EF2-A1919729FA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Search Term</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Y. Nguyen Tan</t>
   </si>
   <si>
-    <t>31.01/24</t>
-  </si>
-  <si>
     <t>IEEE Access</t>
   </si>
   <si>
@@ -332,6 +329,27 @@
   </si>
   <si>
     <t>UNSW-NB15 dataset</t>
+  </si>
+  <si>
+    <t>Advancing Decentralized IoT with Privacy-preserving AI: Harnessing Federated Learning and NLP Techniques</t>
+  </si>
+  <si>
+    <t>Arpita Sarker</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>2023 IEEE International Conference on Artificial Intelligence, Blockchain, and Internet of Things (AIBThings)</t>
+  </si>
+  <si>
+    <t>10.1109/AIBThings58340.2023.10292448</t>
+  </si>
+  <si>
+    <t>This study introduces a cross-platform application built on the Flutter framework that employs federated learning (FL) and natural language processing (NLP) for personalized event discovery. The system includes an NLP-based chatbot and utilizes a second-generation Matrix homeserver known as Dendrite for decentralized communication. The system design is configured to ensure data privacy. The FL model runs on users’ devices, employing data such as browsing history and application usage patterns to build user-interest profiles and provide personalized event suggestions. A practical use case underscores the implementation of end-to-end encrypted communication, indicating the system’s commitment to ensuring privacy and security. The integration of FL and NLP into an IoT context demonstrates a significant advancement in privacy-preserving, personalized applications.</t>
   </si>
 </sst>
 </file>
@@ -339,7 +357,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -373,14 +391,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -399,6 +409,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -408,12 +426,228 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -421,39 +655,184 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF969696"/>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -728,223 +1107,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="32.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="1"/>
-    <col min="15" max="15" width="120.21875" style="7" customWidth="1"/>
-    <col min="16" max="16" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="57" style="1" customWidth="1"/>
-    <col min="20" max="20" width="17.109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="9.109375" style="1"/>
-    <col min="23" max="23" width="15.21875" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="45.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="32" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="32" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="36" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="6"/>
+    <col min="15" max="15" width="120.28515625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="31" style="4" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" style="6" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" style="6" customWidth="1"/>
+    <col min="19" max="19" width="57" style="12" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" style="40" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="4"/>
+    <col min="22" max="22" width="12" style="6" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="6" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="33" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="3" t="s">
+      <c r="S1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="37" t="s">
         <v>16</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="V1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="16">
+        <v>45318</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="15">
+        <v>2024</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="38"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    <row r="3" spans="1:23" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
-        <v>45318</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E3" s="24">
+        <v>45322</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="H3" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="K3" s="23">
+        <v>2023</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="22">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="O3" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" s="23"/>
+    </row>
+    <row r="4" spans="1:23" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="138" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="E4" s="24">
+        <v>45322</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K4" s="23">
         <v>2023</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1">
-        <v>11</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="L4" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="22"/>
+      <c r="N4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="O4" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Unread"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Read"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{30F657E1-F976-457B-97E7-30705BFAEC49}"/>
     <hyperlink ref="N3" r:id="rId2" xr:uid="{3B9485CD-165F-4BC0-A154-0F3E1D604993}"/>
     <hyperlink ref="V3" r:id="rId3" xr:uid="{59566FF4-D4A8-4955-A9A0-353289A10E8B}"/>
+    <hyperlink ref="N4" r:id="rId4" xr:uid="{EDD187A2-9F5D-4EEB-9187-68409543F982}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{314153AD-AECA-42BA-BE96-13F712D1E0C0}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
@@ -965,24 +1427,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating article search file with new notes on artices, and new article information
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Projects\phd\Article Searches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{417DB699-C31E-4E5D-BF54-F5E2B7150162}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>Search Term</t>
   </si>
@@ -54,9 +54,6 @@
     <t xml:space="preserve">First Author </t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Zakaria Abou El Houda</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Limitations</t>
   </si>
   <si>
-    <t>Key Points</t>
-  </si>
-  <si>
     <t>Date Searched</t>
   </si>
   <si>
@@ -150,6 +144,69 @@
     <t>In progress</t>
   </si>
   <si>
+    <t>Main Findings or Points</t>
+  </si>
+  <si>
+    <t>Blockchain</t>
+  </si>
+  <si>
+    <t>Intrusion Detection</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>UNSW-NB15 dataset</t>
+  </si>
+  <si>
+    <t>Advancing Decentralized IoT with Privacy-preserving AI: Harnessing Federated Learning and NLP Techniques</t>
+  </si>
+  <si>
+    <t>Arpita Sarker</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>2023 IEEE International Conference on Artificial Intelligence, Blockchain, and Internet of Things (AIBThings)</t>
+  </si>
+  <si>
+    <t>10.1109/AIBThings58340.2023.10292448</t>
+  </si>
+  <si>
+    <t>This study introduces a cross-platform application built on the Flutter framework that employs federated learning (FL) and natural language processing (NLP) for personalized event discovery. The system includes an NLP-based chatbot and utilizes a second-generation Matrix homeserver known as Dendrite for decentralized communication. The system design is configured to ensure data privacy. The FL model runs on users’ devices, employing data such as browsing history and application usage patterns to build user-interest profiles and provide personalized event suggestions. A practical use case underscores the implementation of end-to-end encrypted communication, indicating the system’s commitment to ensuring privacy and security. The integration of FL and NLP into an IoT context demonstrates a significant advancement in privacy-preserving, personalized applications.</t>
+  </si>
+  <si>
+    <t>Industry 4.0 Enabled Smart Manufacturing: Unleashing the Power of Artificial Intelligence and Blockchain</t>
+  </si>
+  <si>
+    <t>Janmejai Kumar Shah</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>("All Metadata":ai or artificial intelligence) AND ("All Metadata":manufacturing )</t>
+  </si>
+  <si>
+    <t>2023 1st DMIHER International Conference on Artificial Intelligence in Education and Industry 4.0 (IDICAIEI)</t>
+  </si>
+  <si>
+    <t>A new era of manufacturing marked by the convergence of digital technology and physical systems has begun as a result of Industry 4.0's development. This revolution's, smart manufacturing, uses cutting-edge technology like artificial intelligence (AI) and blockchain to promote efficiency, openness, and innovation throughout industrial processes. Using systematic literature review method and thematic analysis, this study looks at the investigation on smart manufacturing industry 4.0, Artificial intelligence and blockchain from 2018 to 2022. The objective of the research is to examine the mutually beneficial interaction between Smart industrial, AI, and Blockchain, outlining how their integration is changing industrial techniques. Furthermore, the study aims to identify potential future trends and research avenues in this area along with development of a conceptual model for future research.</t>
+  </si>
+  <si>
+    <t>10.1109/IDICAIEI58380.2023.10406671</t>
+  </si>
+  <si>
+    <t>10.1109/TITS.2024.3351699</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Intelligent Transportation Systems (ITSs) are transforming the global monitoring of road safety. These systems, including vehicular networks and transportation infrastructure, are vulnerable to </t>
     </r>
@@ -291,11 +348,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>; This system manages reputation data for individual nodes (such as vehicles), guaranteeing the integrity of the FL training process. Experiment results using the UNSW-NB15 dataset show that our proposed framework achieves high accuracy and F1 score (99%) in detecting new threats while ensuring the privacy and reliability of the whole ITS. These results demonstrate the effectiveness of our proposed framework in securing ITS.</t>
-    </r>
-  </si>
-  <si>
-    <t>Main Findings or Points</t>
+      <t xml:space="preserve">; This system manages reputation data for individual nodes (such as vehicles), guaranteeing the integrity of the FL training process. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experiment results using the UNSW-NB15 dataset show that our proposed framework achieves high accuracy and F1 score (99%) in detecting new threats while ensuring the privacy and reliability of the whole ITS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. These results demonstrate the effectiveness of our proposed framework in securing ITS.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -315,41 +389,11 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Edge based framework that used FL and Blockchain  to secure ITS againt intrusions and threats
-• Use of blockchain to maintain reliability and trustworthness of network</t>
-    </r>
-  </si>
-  <si>
-    <t>Blockchain</t>
-  </si>
-  <si>
-    <t>Intrusion Detection</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>UNSW-NB15 dataset</t>
-  </si>
-  <si>
-    <t>Advancing Decentralized IoT with Privacy-preserving AI: Harnessing Federated Learning and NLP Techniques</t>
-  </si>
-  <si>
-    <t>Arpita Sarker</t>
-  </si>
-  <si>
-    <t>NLP</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>2023 IEEE International Conference on Artificial Intelligence, Blockchain, and Internet of Things (AIBThings)</t>
-  </si>
-  <si>
-    <t>10.1109/AIBThings58340.2023.10292448</t>
-  </si>
-  <si>
-    <t>This study introduces a cross-platform application built on the Flutter framework that employs federated learning (FL) and natural language processing (NLP) for personalized event discovery. The system includes an NLP-based chatbot and utilizes a second-generation Matrix homeserver known as Dendrite for decentralized communication. The system design is configured to ensure data privacy. The FL model runs on users’ devices, employing data such as browsing history and application usage patterns to build user-interest profiles and provide personalized event suggestions. A practical use case underscores the implementation of end-to-end encrypted communication, indicating the system’s commitment to ensuring privacy and security. The integration of FL and NLP into an IoT context demonstrates a significant advancement in privacy-preserving, personalized applications.</t>
+• ITS - Intelligent Transport Systems, includes Electronic Toll Collection (ETC), traffic signal synchronisation, and real-time public transport information
+• Use of blockchain to maintain reliability and trustworthness of network
+• Experiments show framework has a high F1 score (99%) in detecting new threats
+• </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -368,6 +412,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -383,14 +433,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -400,19 +442,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -653,128 +697,128 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -782,28 +826,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -821,7 +844,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1107,306 +1130,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="32" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="32" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="36" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="6"/>
-    <col min="15" max="15" width="120.28515625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="31" style="4" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="19.28515625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="57" style="12" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" style="40" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="4"/>
-    <col min="22" max="22" width="12" style="6" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="6" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="45.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="32.81640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.453125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="143.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.7265625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="21.7265625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.26953125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="57" style="6" customWidth="1"/>
+    <col min="19" max="19" width="17.1796875" style="28" customWidth="1"/>
+    <col min="20" max="20" width="12" style="3" customWidth="1"/>
+    <col min="21" max="21" width="15.26953125" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:21" ht="39" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="174.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10">
+        <v>45318</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="9">
+        <v>2024</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="26"/>
+      <c r="T2" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="16">
+        <v>45322</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="K3" s="15">
+        <v>2023</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="14">
+        <v>11</v>
+      </c>
+      <c r="N3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="O3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="15"/>
+    </row>
+    <row r="4" spans="1:21" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="16">
+        <v>45322</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="G4" s="21" t="s">
         <v>44</v>
       </c>
+      <c r="H4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="15">
+        <v>2023</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="14"/>
+      <c r="N4" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
     </row>
-    <row r="2" spans="1:23" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    <row r="5" spans="1:21" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45324</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="16">
-        <v>45318</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="15">
-        <v>2024</v>
-      </c>
-      <c r="L2" s="34" t="s">
+      <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2023</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="38"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="24">
-        <v>45322</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="23">
-        <v>2023</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="22">
-        <v>11</v>
-      </c>
-      <c r="N3" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="23"/>
-    </row>
-    <row r="4" spans="1:23" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="24">
-        <v>45322</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="23">
-        <v>2023</v>
-      </c>
-      <c r="L4" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"Unread"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Read"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Unread"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{30F657E1-F976-457B-97E7-30705BFAEC49}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{3B9485CD-165F-4BC0-A154-0F3E1D604993}"/>
-    <hyperlink ref="V3" r:id="rId3" xr:uid="{59566FF4-D4A8-4955-A9A0-353289A10E8B}"/>
-    <hyperlink ref="N4" r:id="rId4" xr:uid="{EDD187A2-9F5D-4EEB-9187-68409543F982}"/>
+    <hyperlink ref="T3" r:id="rId1" xr:uid="{59566FF4-D4A8-4955-A9A0-353289A10E8B}"/>
+    <hyperlink ref="T2" r:id="rId2" xr:uid="{34A36AD0-F0D1-4437-92DB-76E177EA7BF9}"/>
+    <hyperlink ref="T5" r:id="rId3" xr:uid="{915B563C-74BB-411A-9AB0-B26241DF7AA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{314153AD-AECA-42BA-BE96-13F712D1E0C0}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
@@ -1427,24 +1480,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating notes on Ref 1
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{417DB699-C31E-4E5D-BF54-F5E2B7150162}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{76CE1B24-1540-4C4C-9533-19C66370C147}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>Search Term</t>
   </si>
@@ -370,6 +370,18 @@
       </rPr>
       <t>. These results demonstrate the effectiveness of our proposed framework in securing ITS.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">• The adoption of AI based techniques to secure ITS against threats has been limited due to a lack of realistic and recent data on the types of attacks - without this data, it is difficult to develop AI algorithms to accurately identify and mitigate new threats (i.e. zero-day attacks)
+• </t>
+  </si>
+  <si>
+    <t>Examples Noted in the Work</t>
+  </si>
+  <si>
+    <t>• Traffic data from multiple sensors on roads, traffic cameras, and GPS data from vehicles, could be used to train a golbal model for traffic prediction
+• Blockchain could be used to track the movements of vehicles and ensure authorised vehicles have access to certain areas
+• Blockchain could also be used to store data related to maintenance and repairs, helping ensure vehicles are properly maintained and safe to operate</t>
   </si>
   <si>
     <r>
@@ -394,6 +406,48 @@
 • Experiments show framework has a high F1 score (99%) in detecting new threats
 • </t>
     </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Vehicle networks, knows as Vehicle-to-Everything (V2X) are used to connect vehicles, infrastructure, and padestrians - V2X and ITS have the potential have the potential to improve transportation, but also raise privacy and security concerns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (i.e. collection of location data for individuals)
+• AI based Intrusion Detection Systems (IDS) are used to enhance the security of ITS. There are two types of IDS: (1) network-based IDS, which monitors network traffic, looks for patterns and anomalies that could indicate a threat, and (2) Host-based IDS monitors traffic on a specific computer or device for  for signs of intrusion
+• Blockchain technology could potentially be used to secure ITS by providing a tamper-proof record of transactions and data
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The authors propose a novel Edge-Enabled Framework that uses federated learning and blockchain to secure the ITS against emerging threats (i.e. zero-dat attacks)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>• The use of Edge computing brings security measures closer to the end device, reducing delays in communications and improving the over all security of the system</t>
+    </r>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
 </sst>
 </file>
@@ -403,13 +457,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -461,6 +521,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -470,7 +541,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -694,131 +765,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1130,316 +1236,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="32.81640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.453125" style="25" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="143.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.7265625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="21.7265625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.26953125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="57" style="6" customWidth="1"/>
-    <col min="19" max="19" width="17.1796875" style="28" customWidth="1"/>
-    <col min="20" max="20" width="12" style="3" customWidth="1"/>
-    <col min="21" max="21" width="15.26953125" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="45.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="32.81640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.453125" style="25" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="143.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.7265625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="21.7265625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.26953125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="125.54296875" style="6" customWidth="1"/>
+    <col min="20" max="20" width="78.453125" style="27" customWidth="1"/>
+    <col min="21" max="21" width="107.26953125" style="43" customWidth="1"/>
+    <col min="22" max="22" width="12" style="3" customWidth="1"/>
+    <col min="23" max="23" width="15.26953125" style="3" customWidth="1"/>
+    <col min="24" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="39" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:23" ht="39" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="M1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="N1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="O1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="P1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="Q1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="R1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="S1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="U1" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="W1" s="29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="174.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:23" ht="174.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10">
+      <c r="F2" s="10">
         <v>45318</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9">
+      <c r="L2" s="9">
         <v>2024</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="M2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="8"/>
+      <c r="O2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="9"/>
+      <c r="S2" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="38" t="s">
+      <c r="U2" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:23" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="16">
+      <c r="F3" s="16">
         <v>45322</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="15">
+      <c r="L3" s="15">
         <v>2023</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="M3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="14">
+      <c r="N3" s="14">
         <v>11</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="P3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="39" t="s">
+      <c r="R3" s="15"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="15"/>
+      <c r="W3" s="15"/>
     </row>
-    <row r="4" spans="1:21" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:23" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="16">
+      <c r="F4" s="16">
         <v>45322</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="15">
+      <c r="L4" s="15">
         <v>2023</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="M4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="14"/>
+      <c r="O4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
     </row>
-    <row r="5" spans="1:21" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>45324</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="G5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="H5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>2023</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="M5" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="40" t="s">
+      <c r="V5" s="38" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B1048576">
+  <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Read"</formula>
     </cfRule>
@@ -1451,9 +1584,9 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="T3" r:id="rId1" xr:uid="{59566FF4-D4A8-4955-A9A0-353289A10E8B}"/>
-    <hyperlink ref="T2" r:id="rId2" xr:uid="{34A36AD0-F0D1-4437-92DB-76E177EA7BF9}"/>
-    <hyperlink ref="T5" r:id="rId3" xr:uid="{915B563C-74BB-411A-9AB0-B26241DF7AA8}"/>
+    <hyperlink ref="V3" r:id="rId1" xr:uid="{59566FF4-D4A8-4955-A9A0-353289A10E8B}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{34A36AD0-F0D1-4437-92DB-76E177EA7BF9}"/>
+    <hyperlink ref="V5" r:id="rId3" xr:uid="{915B563C-74BB-411A-9AB0-B26241DF7AA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1464,7 +1597,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
+          <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updating with enw articles
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDF8A6E-1D37-420B-849A-505944BFF61E}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{4267BFDB-7F12-4A8E-9A4A-AA1A2965D563}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>Search Term</t>
   </si>
@@ -557,6 +557,51 @@
       </rPr>
       <t>, consisting of centralised networks such as data centres or cloud servers and will carry out more computationally expensive tasks, such as multi-class classification</t>
     </r>
+  </si>
+  <si>
+    <t>Securing Federated Learning through Blockchain and Explainable AI for Robust Intrusion Detection in IoT Networks</t>
+  </si>
+  <si>
+    <t>IEEE INFOCOM 2023 - IEEE Conference on Computer Communications Workshops (INFOCOM WKSHPS)</t>
+  </si>
+  <si>
+    <t>Federated learning (FL) is a distributed machine learning technique that allows multiple devices or nodes in a network to collaboratively train a machine learning model while keeping their data local to the device. This is particularly useful in the context of the Internet of Things (IoT) systems, where devices may have limited computational resources and may not be able to transmit their data to a central server due to privacy or bandwidth constraints. FL offers privacy protection but remains vulnerable to security and privacy attacks (e.g., Data Poisoning Attacks). To address this issue, in addition to the usual components of an FL system, an explainable FL framework for intrusion detection systems should also include mechanisms for explaining the model's predictions. This can be achieved through the use of techniques such as feature importance, which allows the model to identify the most important input features for a particular prediction. In this context, we propose a novel framework, called FedIoT, that leverages Explainable Artificial Intelligence (XAI) techniques and Blockchain to secure FL-based IDS in the IoT networks. FedIoT uses advanced XAI techniques to identify local model manipulations and mitigate FL-based attacks. Moreover, we propose a blockchain-based approach that uses an efficient reputation scheme that ensures the trustworthiness and reliability of the FL training process. We conduct experiments to validate FedIoT, an FL-based intrusion detection system in IoT networks. Using the UNSW-NB15 dataset, we confirm that FedIoT can effectively detect malicious activities and facilitate efficient FL collaboration among multiple users.</t>
+  </si>
+  <si>
+    <t> 10.1109/INFOCOMWKSHPS57453.2023.10225769</t>
+  </si>
+  <si>
+    <t>Systematic Review on Decentralised Artificial Intelligence and Its Applications</t>
+  </si>
+  <si>
+    <t>Mariya Vincent</t>
+  </si>
+  <si>
+    <t>2023 International Conference on Innovative Data Communication Technologies and Application (ICIDCA)</t>
+  </si>
+  <si>
+    <t>Initially, Artificial Intelligence (AI) models were centralized. This resulted in various challenges. To overcome this challenge, the decentralized or distributed frameworks were developed. Recent advancements in blockchain technology and cryptography have accelerated the decentralization process. Decentralized Artificial Intelligence (DAI) is gaining a significant research attention in recent times. This study reviews various DAI techniques such as Decentralized machine learning frameworks, Federated Learning and Distributed AI marketplaces. In particular, this study focuses on reviewing the recent developments in DAI by analyzing its potential advantages and challenges.</t>
+  </si>
+  <si>
+    <t>10.1109/ICIDCA56705.2023.10100017</t>
+  </si>
+  <si>
+    <t>Edge-Native Intelligence for 6G Communications Driven by Federated Learning: A Survey of Trends and Challenges</t>
+  </si>
+  <si>
+    <t>Mohammad Al-Quraan</t>
+  </si>
+  <si>
+    <t>Federated Learning</t>
+  </si>
+  <si>
+    <t>6G</t>
+  </si>
+  <si>
+    <t>New technological advancements in wireless networks have enlarged the number of connected devices. The unprecedented surge of data volume in wireless systems empowered by artificial intelligence (AI) opens up new horizons for providing ubiquitous data-driven intelligent services. Traditional cloud-centric machine learning (ML)-based services are implemented by centrally collecting datasets and training models. However, this conventional training technique encompasses two challenges: (i) high communication and energy cost and (ii) threatened data privacy. In this article, we introduce a comprehensive survey of the fundamentals and enabling technologies of federated learning (FL), a newly emerging technique coined to bring ML to the edge of wireless networks. Moreover, an extensive study is presented detailing various applications of FL in wireless networks and highlighting their challenges and limitations. The efficacy of FL is further explored with emerging prospective beyond fifth-generation (B5G) and sixth-generation (6G) communication systems. This survey aims to provide an overview of the state-of-the-art FL applications in key wireless technologies that will serve as a foundation to establish a firm understanding of the topic. Lastly, we offer a road forward for future research directions.</t>
+  </si>
+  <si>
+    <t>10.1109/TETCI.2023.3251404</t>
   </si>
 </sst>
 </file>
@@ -900,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1013,9 +1058,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1036,6 +1078,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1346,11 +1400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -1367,22 +1421,22 @@
     <col min="10" max="10" width="32.81640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.453125" style="25" customWidth="1"/>
+    <col min="13" max="13" width="43.90625" style="25" customWidth="1"/>
     <col min="14" max="14" width="8.81640625" style="2" customWidth="1"/>
     <col min="15" max="15" width="143.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.7265625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="43.81640625" style="2" customWidth="1"/>
     <col min="17" max="17" width="21.7265625" style="3" customWidth="1"/>
     <col min="18" max="18" width="19.26953125" style="3" customWidth="1"/>
     <col min="19" max="19" width="125.54296875" style="6" customWidth="1"/>
     <col min="20" max="20" width="78.453125" style="27" customWidth="1"/>
-    <col min="21" max="21" width="107.26953125" style="42" customWidth="1"/>
+    <col min="21" max="21" width="107.26953125" style="41" customWidth="1"/>
     <col min="22" max="22" width="12" style="3" customWidth="1"/>
     <col min="23" max="23" width="15.26953125" style="3" customWidth="1"/>
     <col min="24" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="39" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="28" t="s">
@@ -1442,7 +1496,7 @@
       <c r="T1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="39" t="s">
         <v>60</v>
       </c>
       <c r="V1" s="29" t="s">
@@ -1452,8 +1506,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="299" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="2" spans="1:23" ht="128" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1501,13 +1555,13 @@
       </c>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="45" t="s">
+      <c r="S2" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="U2" s="43" t="s">
+      <c r="U2" s="42" t="s">
         <v>61</v>
       </c>
       <c r="V2" s="36" t="s">
@@ -1518,7 +1572,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="40">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -1570,14 +1624,14 @@
       <c r="R3" s="15"/>
       <c r="S3" s="18"/>
       <c r="T3" s="26"/>
-      <c r="U3" s="41"/>
+      <c r="U3" s="40"/>
       <c r="V3" s="37" t="s">
         <v>11</v>
       </c>
       <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:23" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="40">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -1627,57 +1681,212 @@
       <c r="R4" s="15"/>
       <c r="S4" s="18"/>
       <c r="T4" s="26"/>
-      <c r="U4" s="41"/>
+      <c r="U4" s="40"/>
       <c r="V4" s="15"/>
       <c r="W4" s="15"/>
     </row>
-    <row r="5" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+    <row r="5" spans="1:23" ht="78" x14ac:dyDescent="0.35">
+      <c r="A5" s="40">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="16">
         <v>45324</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="15">
         <v>2023</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="N5" s="14"/>
+      <c r="O5" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="V5" s="38" t="s">
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" s="15"/>
+    </row>
+    <row r="6" spans="1:23" ht="130" x14ac:dyDescent="0.35">
+      <c r="A6" s="40">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="16">
+        <v>45326</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="15">
+        <v>2023</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="W6" s="15"/>
+    </row>
+    <row r="7" spans="1:23" ht="52" x14ac:dyDescent="0.35">
+      <c r="A7" s="40">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="16">
+        <v>45326</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="15">
+        <v>2023</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="14"/>
+      <c r="O7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="W7" s="15"/>
+    </row>
+    <row r="8" spans="1:23" ht="104" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45327</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="V8" s="45" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1697,9 +1906,12 @@
     <hyperlink ref="V3" r:id="rId1" xr:uid="{59566FF4-D4A8-4955-A9A0-353289A10E8B}"/>
     <hyperlink ref="V2" r:id="rId2" xr:uid="{34A36AD0-F0D1-4437-92DB-76E177EA7BF9}"/>
     <hyperlink ref="V5" r:id="rId3" xr:uid="{915B563C-74BB-411A-9AB0-B26241DF7AA8}"/>
+    <hyperlink ref="V7" r:id="rId4" xr:uid="{6D0C5EBC-679E-474E-BAAE-E43E805F57B6}"/>
+    <hyperlink ref="V6" r:id="rId5" xr:uid="{710D2BA7-402F-477C-A7F3-CC9E1508FFE3}"/>
+    <hyperlink ref="V8" r:id="rId6" xr:uid="{78711401-3387-441B-B66F-C1BE8EE6498A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Updated sheet with more article info
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{4267BFDB-7F12-4A8E-9A4A-AA1A2965D563}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA6258A5-82E5-4C95-9FA4-20B046AF9D21}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Main Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Terms" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Table'!$H$1:$H$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>Search Term</t>
   </si>
@@ -602,6 +603,48 @@
   </si>
   <si>
     <t>10.1109/TETCI.2023.3251404</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Emerging Topics in Computational Intelligence</t>
+  </si>
+  <si>
+    <t>("All Metadata":ai or artificial intelligence) AND ("All Metadata":manufacturing) AND ("All Metadata":federated learning)</t>
+  </si>
+  <si>
+    <t>A Federated Learning Framework for Enforcing Traceability in Manufacturing Processes</t>
+  </si>
+  <si>
+    <t>Isaak Kavasidis</t>
+  </si>
+  <si>
+    <t>The plethora of available data in various manufacturing facilities has boosted the adoption of various data analytics methods, which are tailored to a wide range of operations and tasks. However, fragmentation of data, in the sense that chunks of data could possibly be distributed in geographically sparse areas, hampers the generation of better and more accurate intelligent models that would otherwise benefit from the larger quantities of available data which are derived from various operations taking place at different locations of a manufacturing process. Moreover, in regulated industrial sectors, such as in the medical and the pharmaceutical fields, sector-specific legislation imposes strict criteria and rules for the privacy, maintenance and long-term storage of data. Process reproducibility is often an essential requirement in these regulated industrial sectors, and this issue could be supported by AI models which can be applied to enforce traceability, auditability and integrity of every initial, intermediate and final piece of data used during the AI model training process. In this respect, blockchain technologies could be potentially also useful for enabling and enforcing such requirements. In this paper, we present a multi-blockchain-based platform integrated with federated learning functionalities to train global AI (deep learning) models. The proposed platform maintains an audit trail of all information pertaining the training process using a set of blockchains in order to ensure the training process’s immutability. The applicability of the proposed framework has been validated on three tasks by applying three state-of-the-art federated learning algorithms on an industrial pharmaceutical dataset based on two manufacturing lines, achieving promising in terms of both generalizability and convergence time.</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2023.3282316</t>
+  </si>
+  <si>
+    <t>Blockchain Assisted Data Edge Verification With Consensus Algorithm for Machine Learning Assisted IoT</t>
+  </si>
+  <si>
+    <t>Thavavel Vaiyapuri</t>
+  </si>
+  <si>
+    <t>Internet of Things (IoT) devices are becoming increasingly ubiquitous in daily life. They are utilized in various sectors like healthcare, manufacturing, and transportation. The main challenges related to IoT devices are the potential for faults to occur and their reliability. In classical IoT fault detection, the client device must upload raw information to the central server for the training model, which can reveal sensitive business information. Blockchain (BC) technology and a fault detection algorithm are applied to overcome these challenges. Generally, the fusion of BC technology and fault detection algorithms can give a secure and more reliable IoT ecosystem. Therefore, this study develops a new Blockchain Assisted Data Edge Verification with Consensus Algorithm for Machine Learning (BDEV-CAML) technique for IoT Fault Detection purposes. The presented BDEV-CAML technique integrates the benefits of blockchain, IoT, and ML models to enhance the IoT network’s trustworthiness, efficacy, and security. In BC technology, IoT devices that possess a significant level of decentralized decision-making capability can attain a consensus on the efficiency of intrablock transactions. For fault detection in the IoT network, the deep directional gated recurrent unit (DBiGRU) model is used. Finally, the African vulture optimization algorithm (AVOA) technique is utilized for the optimal hyperparameter tuning of the DBiGRU model, which helps in improving the fault detection rate. A detailed set of experiments were carried out to highlight the enhanced performance of the BDEV-CAML algorithm. The comprehensive experimental results stated the improved performance of the BDEV-CAML technique over other existing models with maximum accuracy of 99.6%.</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2023.3280798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abbrev. </t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
   </si>
 </sst>
 </file>
@@ -1400,11 +1443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -1435,7 +1478,7 @@
     <col min="24" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="43" t="s">
         <v>62</v>
       </c>
@@ -1799,7 +1842,7 @@
       </c>
       <c r="W6" s="15"/>
     </row>
-    <row r="7" spans="1:23" ht="52" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="40">
         <v>6</v>
       </c>
@@ -1880,6 +1923,18 @@
       <c r="I8" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="J8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2023</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>79</v>
+      </c>
       <c r="O8" s="7" t="s">
         <v>77</v>
       </c>
@@ -1887,6 +1942,106 @@
         <v>78</v>
       </c>
       <c r="V8" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="143" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45329</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="3">
+        <v>2023</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="2">
+        <v>11</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V9" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="100.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="4">
+        <v>45329</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="2">
+        <v>11</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="V10" s="45" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1909,9 +2064,11 @@
     <hyperlink ref="V7" r:id="rId4" xr:uid="{6D0C5EBC-679E-474E-BAAE-E43E805F57B6}"/>
     <hyperlink ref="V6" r:id="rId5" xr:uid="{710D2BA7-402F-477C-A7F3-CC9E1508FFE3}"/>
     <hyperlink ref="V8" r:id="rId6" xr:uid="{78711401-3387-441B-B66F-C1BE8EE6498A}"/>
+    <hyperlink ref="V9" r:id="rId7" xr:uid="{C79D88A9-23C4-427E-9BFC-7118B53FAAEC}"/>
+    <hyperlink ref="V10" r:id="rId8" xr:uid="{1A28BA75-CA82-4D9C-9E4D-B8CCE410213E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1928,6 +2085,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EBCE0F-3CAE-4AF1-964E-E55D8D597B13}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BAB843-83FA-47C8-832D-D9EB97543B0C}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Getting files up to date
</commit_message>
<xml_diff>
--- a/Article Searches/article_search.xlsx
+++ b/Article Searches/article_search.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{356B91B2-6CBB-4183-8E7F-D198930D329E}"/>
+  <xr:revisionPtr revIDLastSave="273" documentId="13_ncr:1_{90E70C55-5A94-41D9-8BD2-2F044D1A5E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C62E19F4-EB22-47A5-91A1-84A0B0F3ED30}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1440" yWindow="-14760" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Table'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -32,16 +43,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
+    <t>Ref</t>
+  </si>
+  <si>
     <t>Title</t>
   </si>
   <si>
+    <t xml:space="preserve">First Author </t>
+  </si>
+  <si>
     <t>Database</t>
   </si>
   <si>
+    <t>Date Searched</t>
+  </si>
+  <si>
     <t>Pub. Year</t>
   </si>
   <si>
     <t>Journal</t>
+  </si>
+  <si>
+    <t>Vol.</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Purpose/Research Gap</t>
+  </si>
+  <si>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>Main Findings or Points</t>
+  </si>
+  <si>
+    <t>Limitations</t>
+  </si>
+  <si>
+    <t>Examples Noted in the Work</t>
+  </si>
+  <si>
+    <t>Mendeley Link</t>
+  </si>
+  <si>
+    <t>Dataset</t>
   </si>
   <si>
     <t>Blockchain-Enabled Federated learning
@@ -49,9 +96,6 @@
 in Vehicular Edge Computing</t>
   </si>
   <si>
-    <t xml:space="preserve">First Author </t>
-  </si>
-  <si>
     <t>Zakaria Abou El Houda</t>
   </si>
   <si>
@@ -61,172 +105,18 @@
     <t>IEEE Transactions on Intelligent Transportation Systems</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Methodology</t>
-  </si>
-  <si>
-    <t>Purpose/Research Gap</t>
-  </si>
-  <si>
-    <t>Limitations</t>
-  </si>
-  <si>
-    <t>Date Searched</t>
-  </si>
-  <si>
-    <t>A Transfer Learning Approach to Breast Cancer Classification in a Federated Learning Framework</t>
-  </si>
-  <si>
-    <t>Y. Nguyen Tan</t>
-  </si>
-  <si>
-    <t>IEEE Access</t>
-  </si>
-  <si>
-    <t>DOI</t>
-  </si>
-  <si>
-    <t>10.1109/ACCESS.2023.3257562</t>
-  </si>
-  <si>
-    <t>Vol.</t>
-  </si>
-  <si>
-    <t>Mendeley Link</t>
-  </si>
-  <si>
-    <t>Read</t>
-  </si>
-  <si>
-    <t>Unread</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>Main Findings or Points</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>UNSW-NB15 dataset</t>
-  </si>
-  <si>
-    <t>Advancing Decentralized IoT with Privacy-preserving AI: Harnessing Federated Learning and NLP Techniques</t>
-  </si>
-  <si>
-    <t>Arpita Sarker</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>2023 IEEE International Conference on Artificial Intelligence, Blockchain, and Internet of Things (AIBThings)</t>
-  </si>
-  <si>
-    <t>10.1109/AIBThings58340.2023.10292448</t>
-  </si>
-  <si>
-    <t>Industry 4.0 Enabled Smart Manufacturing: Unleashing the Power of Artificial Intelligence and Blockchain</t>
-  </si>
-  <si>
-    <t>Janmejai Kumar Shah</t>
-  </si>
-  <si>
-    <t>2023 1st DMIHER International Conference on Artificial Intelligence in Education and Industry 4.0 (IDICAIEI)</t>
-  </si>
-  <si>
-    <t>10.1109/IDICAIEI58380.2023.10406671</t>
-  </si>
-  <si>
     <t>10.1109/TITS.2024.3351699</t>
   </si>
   <si>
-    <t xml:space="preserve">• The adoption of AI based techniques to secure ITS against threats has been limited due to a lack of realistic and recent data on the types of attacks - without this data, it is difficult to develop AI algorithms to accurately identify and mitigate new threats (i.e. zero-day attacks)
-• </t>
-  </si>
-  <si>
-    <t>Examples Noted in the Work</t>
-  </si>
-  <si>
-    <t>• Traffic data from multiple sensors on roads, traffic cameras, and GPS data from vehicles, could be used to train a golbal model for traffic prediction
-• Blockchain could be used to track the movements of vehicles and ensure authorised vehicles have access to certain areas
-• Blockchain could also be used to store data related to maintenance and repairs, helping ensure vehicles are properly maintained and safe to operate</t>
-  </si>
-  <si>
-    <t>Ref</t>
-  </si>
-  <si>
-    <t>Securing Federated Learning through Blockchain and Explainable AI for Robust Intrusion Detection in IoT Networks</t>
-  </si>
-  <si>
-    <t>IEEE INFOCOM 2023 - IEEE Conference on Computer Communications Workshops (INFOCOM WKSHPS)</t>
-  </si>
-  <si>
-    <t> 10.1109/INFOCOMWKSHPS57453.2023.10225769</t>
-  </si>
-  <si>
-    <t>Systematic Review on Decentralised Artificial Intelligence and Its Applications</t>
-  </si>
-  <si>
-    <t>Mariya Vincent</t>
-  </si>
-  <si>
-    <t>2023 International Conference on Innovative Data Communication Technologies and Application (ICIDCA)</t>
-  </si>
-  <si>
-    <t>10.1109/ICIDCA56705.2023.10100017</t>
-  </si>
-  <si>
-    <t>Edge-Native Intelligence for 6G Communications Driven by Federated Learning: A Survey of Trends and Challenges</t>
-  </si>
-  <si>
-    <t>Mohammad Al-Quraan</t>
-  </si>
-  <si>
-    <t>10.1109/TETCI.2023.3251404</t>
-  </si>
-  <si>
-    <t>IEEE Transactions on Emerging Topics in Computational Intelligence</t>
-  </si>
-  <si>
-    <t>A Federated Learning Framework for Enforcing Traceability in Manufacturing Processes</t>
-  </si>
-  <si>
-    <t>Isaak Kavasidis</t>
-  </si>
-  <si>
-    <t>10.1109/ACCESS.2023.3282316</t>
-  </si>
-  <si>
-    <t>Blockchain Assisted Data Edge Verification With Consensus Algorithm for Machine Learning Assisted IoT</t>
-  </si>
-  <si>
-    <t>Thavavel Vaiyapuri</t>
-  </si>
-  <si>
-    <t>10.1109/ACCESS.2023.3280798</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abbrev. </t>
-  </si>
-  <si>
-    <t>Meaning</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Internet of Things</t>
-  </si>
-  <si>
     <t>Develop framework to secure ITS against emerging threats using FL and blockchain</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">• Edge based framework that used FL and Blockchain  to secure ITS againt intrusions and threats. ITS - Intelligent Transport Systems, includes Electronic Toll Collection (ETC), traffic signal synchronisation, and real-time public transport information
 • Use of blockchain to maintain reliability and trustworthness of network
 • Experiments show framework has a high F1 score (99%) in detecting new threats
@@ -242,8 +132,6 @@
         <sz val="10"/>
         <color rgb="FFFF3300"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Blockchain ensures the trustworthiness and reliability of the FL training process
 </t>
@@ -251,61 +139,42 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">• The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">UNSW-NB15 dataset contains well-known attacks and malwarewas used
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">• The UNSW-NB15 dataset contains well-known attacks and malwarewas used
+• </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Proposed framework has 3 tiers:</t>
+      </rPr>
+      <t xml:space="preserve">Proposed framework has 3 tiers:
+</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-• </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>Tiers 1</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">: nodes in the </t>
     </r>
@@ -314,15 +183,14 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>vehicular network</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">, such as sensors in vehicles and comms systems. This node collects data and carries out initial processing using onboard processors and resources
 • </t>
@@ -332,15 +200,14 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>Tier 2</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">: the </t>
     </r>
@@ -349,15 +216,14 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>edge computing layer</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> consists of intermediate processing nodes located closer to the edge of the network, such as traffic intersections or on-road infrastructure - these nodes prefore more complex tasks, such as classification, using more powerful resources
 • </t>
@@ -367,15 +233,14 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>Tier 3</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">: the </t>
     </r>
@@ -384,46 +249,43 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>cloud tier</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, consisting of centralised networks such as data centres or cloud servers and will carry out more computationally expensive tasks, such as multi-class classification</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>•</t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>, consisting of centralised networks such as data centres or cloud servers and will carry out more computationally expensive tasks, such as multi-class classification
+•</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> Blockchain system used to manage reputations of nodes (e.g. cars)</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">• The adoption of AI based techniques to secure ITS against threats has been limited due to a lack of realistic and recent data on the types of attacks - without this data, it is difficult to develop AI algorithms to accurately identify and mitigate new threats (i.e. zero-day attacks)
+• </t>
+  </si>
+  <si>
+    <t>• Traffic data from multiple sensors on roads, traffic cameras, and GPS data from vehicles, could be used to train a golbal model for traffic prediction
+• Blockchain could be used to track the movements of vehicles and ensure authorised vehicles have access to certain areas
+• Blockchain could also be used to store data related to maintenance and repairs, helping ensure vehicles are properly maintained and safe to operate</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>UNSW-NB15 dataset</t>
+  </si>
+  <si>
     <t>Adaptive asynchronous federated learning</t>
   </si>
   <si>
@@ -437,6 +299,117 @@
   </si>
   <si>
     <t>10.1016/j.future.2023.11.001</t>
+  </si>
+  <si>
+    <t>A Transfer Learning Approach to Breast Cancer Classification in a Federated Learning Framework</t>
+  </si>
+  <si>
+    <t>Y. Nguyen Tan</t>
+  </si>
+  <si>
+    <t>IEEE Access</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2023.3257562</t>
+  </si>
+  <si>
+    <t>Advancing Decentralized IoT with Privacy-preserving AI: Harnessing Federated Learning and NLP Techniques</t>
+  </si>
+  <si>
+    <t>Arpita Sarker</t>
+  </si>
+  <si>
+    <t>2023 IEEE International Conference on Artificial Intelligence, Blockchain, and Internet of Things (AIBThings)</t>
+  </si>
+  <si>
+    <t>10.1109/AIBThings58340.2023.10292448</t>
+  </si>
+  <si>
+    <t>Industry 4.0 Enabled Smart Manufacturing: Unleashing the Power of Artificial Intelligence and Blockchain</t>
+  </si>
+  <si>
+    <t>Janmejai Kumar Shah</t>
+  </si>
+  <si>
+    <t>2023 1st DMIHER International Conference on Artificial Intelligence in Education and Industry 4.0 (IDICAIEI)</t>
+  </si>
+  <si>
+    <t>10.1109/IDICAIEI58380.2023.10406671</t>
+  </si>
+  <si>
+    <t>Securing Federated Learning through Blockchain and Explainable AI for Robust Intrusion Detection in IoT Networks</t>
+  </si>
+  <si>
+    <t>IEEE INFOCOM 2023 - IEEE Conference on Computer Communications Workshops (INFOCOM WKSHPS)</t>
+  </si>
+  <si>
+    <t> 10.1109/INFOCOMWKSHPS57453.2023.10225769</t>
+  </si>
+  <si>
+    <t>Systematic Review on Decentralised Artificial Intelligence and Its Applications</t>
+  </si>
+  <si>
+    <t>Mariya Vincent</t>
+  </si>
+  <si>
+    <t>2023 International Conference on Innovative Data Communication Technologies and Application (ICIDCA)</t>
+  </si>
+  <si>
+    <t>10.1109/ICIDCA56705.2023.10100017</t>
+  </si>
+  <si>
+    <t>Edge-Native Intelligence for 6G Communications Driven by Federated Learning: A Survey of Trends and Challenges</t>
+  </si>
+  <si>
+    <t>Mohammad Al-Quraan</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Emerging Topics in Computational Intelligence</t>
+  </si>
+  <si>
+    <t>10.1109/TETCI.2023.3251404</t>
+  </si>
+  <si>
+    <t>A Federated Learning Framework for Enforcing Traceability in Manufacturing Processes</t>
+  </si>
+  <si>
+    <t>Isaak Kavasidis</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2023.3282316</t>
+  </si>
+  <si>
+    <t>Blockchain Assisted Data Edge Verification With Consensus Algorithm for Machine Learning Assisted IoT</t>
+  </si>
+  <si>
+    <t>Thavavel Vaiyapuri</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2023.3280798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abbrev. </t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Unread</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -446,7 +419,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,30 +468,31 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF3300"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -745,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -837,7 +811,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -854,6 +828,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1145,93 +1122,93 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="J2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1"/>
-    <col min="2" max="2" width="45.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.88671875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="43.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="28.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="125.5546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="78.44140625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="107.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1"/>
+    <col min="2" max="2" width="45.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.85546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="28.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="125.5703125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="78.42578125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="107.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="12" style="3" customWidth="1"/>
-    <col min="16" max="16" width="15.21875" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="9.21875" style="1"/>
+    <col min="16" max="16" width="15.28515625" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="48.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="48.4" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="23" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="M1" s="24" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="270" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="270" customHeight="1">
       <c r="A2" s="33">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E2" s="8">
         <v>45318</v>
@@ -1240,44 +1217,44 @@
         <v>2024</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="K2" s="7"/>
-      <c r="L2" s="31" t="s">
-        <v>63</v>
+      <c r="L2" s="37" t="s">
+        <v>22</v>
       </c>
       <c r="M2" s="27" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N2" s="30" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="270" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="270" customHeight="1">
       <c r="A3" s="33">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="E3" s="8">
         <v>45331</v>
@@ -1286,13 +1263,13 @@
         <v>2024</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="H3" s="6">
         <v>152</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1300,22 +1277,22 @@
       <c r="M3" s="27"/>
       <c r="N3" s="30"/>
       <c r="O3" s="36" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:16" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="151.5" customHeight="1">
       <c r="A4" s="29">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E4" s="12">
         <v>45322</v>
@@ -1324,13 +1301,13 @@
         <v>2023</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H4" s="10">
         <v>11</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -1338,22 +1315,22 @@
       <c r="M4" s="17"/>
       <c r="N4" s="29"/>
       <c r="O4" s="26" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="111.75" customHeight="1">
       <c r="A5" s="29">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E5" s="12">
         <v>45322</v>
@@ -1362,11 +1339,11 @@
         <v>2023</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -1376,18 +1353,18 @@
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="41.45">
       <c r="A6" s="29">
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E6" s="12">
         <v>45324</v>
@@ -1396,11 +1373,11 @@
         <v>2023</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -1408,22 +1385,22 @@
       <c r="M6" s="17"/>
       <c r="N6" s="29"/>
       <c r="O6" s="26" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="41.45">
       <c r="A7" s="29">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E7" s="12">
         <v>45326</v>
@@ -1432,11 +1409,11 @@
         <v>2023</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -1444,22 +1421,22 @@
       <c r="M7" s="17"/>
       <c r="N7" s="29"/>
       <c r="O7" s="35" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" ht="84.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="84.4" customHeight="1">
       <c r="A8" s="29">
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E8" s="12">
         <v>45326</v>
@@ -1468,11 +1445,11 @@
         <v>2023</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1480,22 +1457,22 @@
       <c r="M8" s="17"/>
       <c r="N8" s="29"/>
       <c r="O8" s="35" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="41.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E9" s="4">
         <v>45327</v>
@@ -1504,27 +1481,27 @@
         <v>2023</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="27.6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4">
         <v>45329</v>
@@ -1533,45 +1510,45 @@
         <v>2023</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2">
         <v>11</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="100.5" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4">
         <v>45329</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H11" s="2">
         <v>11</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1599,28 +1576,28 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1636,24 +1613,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>